<commit_message>
Spreading other options. Q25 to fix (Académicien & Ancien Académicien)
</commit_message>
<xml_diff>
--- a/data/ac_survey.xlsx
+++ b/data/ac_survey.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="330">
   <si>
     <t>Horodateur</t>
   </si>
@@ -950,6 +950,66 @@
   </si>
   <si>
     <t>Local, Végétarien</t>
+  </si>
+  <si>
+    <t>On a un fort potentiel d'action à l'échelle individuelle, Je suis prêt à baisser mon niveau de vie si cette baisse s'opère pour les autres également, Je suis prêt à baisser mon niveau de vie même si cette baisse ne s'opère pas pour les autres, Une transition écologique efficace peut se faire dans un cadre démocratique, Pour agir efficacement, il faut hiérarchiser les problèmes (perte de biodiversité, dérèglement climatique etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On ne peut pas parler de mouvement religieux dans le sens où même si certains livre font foi dans le mouvement, on ne suit aucun écrit à la règle sans réflexions. </t>
+  </si>
+  <si>
+    <t>Local, Bio majoritairement (+ de 50% de ce que tu manges chez toi)</t>
+  </si>
+  <si>
+    <t>Je comprend qu'il y ait des personnes climatosceptiques au sein de la population, Je suis prêt à baisser mon niveau de vie même si cette baisse ne s'opère pas pour les autres</t>
+  </si>
+  <si>
+    <t>Ingénierie industrielle / énergétique</t>
+  </si>
+  <si>
+    <t>Cela ressemble énormément à un dogme, mais j'y suis sensible malgré cette impression. Je trouve que nous sommes poussés à nous éloigner de nos ressentis par la société. En prenant le temps de regarder en dehors du cadre imposé par les normes sociales, les enjeux climatique me semble être une évidence.</t>
+  </si>
+  <si>
+    <t>Livres, une intuition venue dès la naissance, grande sensibilité pour les animaux et la protection de la nature, sans vraiment lire de documents scientifiques. quelques documentaires grand public (la planète bleue, la planète blanche)</t>
+  </si>
+  <si>
+    <t>mélange de tristesse et d'excitation de qu'est ce qu'on va faire ensuite</t>
+  </si>
+  <si>
+    <t>Je suis prêt à baisser mon niveau de vie si cette baisse s'opère pour les autres également, Je suis prêt à baisser mon niveau de vie même si cette baisse ne s'opère pas pour les autres, Une transition écologique efficace peut se faire dans un cadre démocratique, Pour agir efficacement, il faut hiérarchiser les problèmes (perte de biodiversité, dérèglement climatique etc.)</t>
+  </si>
+  <si>
+    <t>Une réaction de personnes ne voulant pas toucher à leur mode de vie, Problème d'éducation et/ou d'information, une fuite pour ne pas faire face au problème</t>
+  </si>
+  <si>
+    <t>Le militantisme écologique ne cherche pas à rassembler des personnes dans une foi en un dieu mais de faire prendre conscience d'une situation tangible grave et d'un comportement global non adapté. Je pense néanmoins qu'il peut faire appel à des notions communes à la religion comme le respect du vivant.</t>
+  </si>
+  <si>
+    <t>Académicien, investie dans le Pôle culturel</t>
+  </si>
+  <si>
+    <t>On a un fort potentiel d'action à l'échelle individuelle, Je comprend qu'il y ait des personnes climatosceptiques au sein de la population, Une transition écologique efficace peut se faire dans un cadre démocratique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une opinion différente, mais qui a une probabilité d'être juste, Un terme assez condescendant pour catégoriser ceux qui remettent en question le caractère majoritairement anthropique du changement climatique </t>
+  </si>
+  <si>
+    <t>Je fais profil bas. Trop en parler, c'est devenir prêcheur, et donc desservir la cause., Je donne une conférence sur les enjeux énergie-climat (hi hi hi), Je montre l'exemple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dogme religieux fermé aux opinions contraires et qui les rejette fortement </t>
+  </si>
+  <si>
+    <t>Conférences (Jancovici, Bihouix etc.), Le bouche à oreille (conférences, rencontres, associations...)</t>
+  </si>
+  <si>
+    <t>Je partage des liens sur les réseaux sociaux, Je donne une conférence sur les enjeux énergie-climat (hi hi hi), Je leur fait à manger vegan (et c'est bon niark niark niark)</t>
+  </si>
+  <si>
+    <t>Je trouve que les personnes écolos ont des références assez variées et sont touchées par le réchauffement climatique pour différentes causes et à différents dégrés</t>
+  </si>
+  <si>
+    <t>Bio majoritairement (+ de 50% de ce que tu manges chez toi), Végétalien</t>
   </si>
 </sst>
 </file>
@@ -5534,6 +5594,501 @@
         <v>59</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>43543.66878363426</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K56" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L56" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="M56" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="N56" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="O56" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T56" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="U56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X56" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y56" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="Z56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB56" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>43543.80020091435</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K57" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L57" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="M57" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N57" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="O57" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T57" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="U57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W57" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="X57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB57" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>43543.84074148149</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K58" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="L58" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="M58" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="N58" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="O58" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T58" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="U58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z58" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB58" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>43543.94531111111</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D59" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K59" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="L59" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="M59" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N59" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="O59" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T59" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W59" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="X59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB59" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2">
+        <v>43544.06678005787</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="K60" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L60" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="M60" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="N60" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="O60" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T60" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z60" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>43544.51922133102</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K61" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L61" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="M61" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N61" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="O61" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T61" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="U61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W61" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="X61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y61" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z61" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB61" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add plots of factors and begin to deal with logical values
</commit_message>
<xml_diff>
--- a/data/ac_survey.xlsx
+++ b/data/ac_survey.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="340">
   <si>
     <t>Horodateur</t>
   </si>
@@ -1010,6 +1010,39 @@
   </si>
   <si>
     <t>Bio majoritairement (+ de 50% de ce que tu manges chez toi), Végétalien</t>
+  </si>
+  <si>
+    <t>Conférences (Jancovici, Bihouix etc.), Articles de vulgarisation &amp; blogs, Vidéos Youtube de vulgarisation</t>
+  </si>
+  <si>
+    <t>On a un fort potentiel d'action à l'échelle individuelle, Je comprend qu'il y ait des personnes climatosceptiques au sein de la population, Je suis prêt à baisser mon niveau de vie même si cette baisse ne s'opère pas pour les autres, Une transition écologique efficace peut se faire dans un cadre démocratique</t>
+  </si>
+  <si>
+    <t>En effet, on m'a déjà fait la remarque que dans mon argumentation, je souhaite presque cet effondrement. Tous mes arguments et les réponses vont vers ça. Comme pour le mouvement écolo des années 70 qui était déjà aussi alarmiste.
+C'est vrai que pour ma part en tout cas, je sens que dans la crise écolo et sociale, il y a la confirmation à mon intuition/constat personnel que le système est mauvais et qu'il faut le changer. Intuition que j'ai depuis toujours ou presque. Et là ces constats alarmistes et scientifiques me donnent raison, donc j'y vais.
+Et j'y vais d'autant mieux qu'on se retrouve, qu'on construit/réfléchis ensemble, bref qu'on retrouve un lien social fort autour d'une thématique qui est très forte chez nous, et donc qui recréé un sentiment d'appartenance à un groupe, une communauté, etc. Ce qui est un sentiment génial et rassurant, d'autant plus en ces temps où la famille est moins forte/nombreuse, les amitiés moins durables ou solides...
+Et dans ce confortable sentiment d'appartenance, où on se reconnaît entre nous, certains peuvent devenir dogmatique et "dériver"vers une opposition ou un besoin de se définir contre les autres.</t>
+  </si>
+  <si>
+    <t>Conférences (Jancovici, Bihouix etc.), Livres, Cours</t>
+  </si>
+  <si>
+    <t>Energie</t>
+  </si>
+  <si>
+    <t>Une réaction de personnes ne voulant pas toucher à leur mode de vie, Problème d'éducation et/ou d'information, Des personnes constituées d'un système de valeurs remis en question quand il s'agit de parler de transition écologique, énergétique, de sobriété, de low tech</t>
+  </si>
+  <si>
+    <t>Il est vrai que l'on fait confiance aux scientifiques et que l'on partage facilement des articles sur le sujet du dérèglement climatique parfois aveuglement. cependant chacun a son échelle et même un européen voit un peu les impacts nocifs : pollution, vague de chaleur, inondation, feu de foret, perte de biodiversité, artificialisation massive, pollution plastique dans les cous d'eau.. donc même si on n'est pas scientifique et que l'on n'a pas tous accès à l'information exacte, on peut faire état de la situation sans l'avoir entendu par un gourou</t>
+  </si>
+  <si>
+    <t>Soulagement</t>
+  </si>
+  <si>
+    <t>On peut augmenter le pouvoir d'achat en France tout en se limitant à une augmentation de la T° moyenne de 2°C, Je suis prêt à baisser mon niveau de vie même si cette baisse ne s'opère pas pour les autres</t>
+  </si>
+  <si>
+    <t>Je ressens profondément le fait d'être une bulle, une bulle confortable et consensuelle, vis à vis de mon militantisme écologique. Je pense que j'ai une forme de fracture dans mon esprit que les contestations sociales représentées par le mouvement des gilets jaunes contribuent à rendre plus intelligibles, que j'arrive de mieux à mieux à appréhender et à verbaliser. Ça me donne le sentiment que je me suis trompée de combat avec le militantisme écologique et que la crise sociale est bien plus urgente pour l'humanité.</t>
   </si>
 </sst>
 </file>
@@ -6089,6 +6122,415 @@
         <v>59</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>43545.438302905095</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D62" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K62" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L62" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="M62" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N62" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="O62" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T62" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="U62" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W62" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="X62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB62" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2">
+        <v>43545.490691018524</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D63" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K63" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="L63" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="M63" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N63" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="O63" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T63" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="U63" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W63" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="X63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y63" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB63" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2">
+        <v>43545.62710184028</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K64" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="L64" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="M64" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="N64" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="O64" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T64" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="U64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W64" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="X64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB64" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2">
+        <v>43547.43574328704</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="K65" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="L65" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="M65" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N65" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="O65" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T65" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="U65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z65" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB65" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2">
+        <v>43547.54042091435</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D66" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K66" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="L66" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="M66" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N66" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="O66" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="R66" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="S66" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T66" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="U66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W66" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y66" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB66" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify some file, add MCA
</commit_message>
<xml_diff>
--- a/data/ac_survey.xlsx
+++ b/data/ac_survey.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="344">
   <si>
     <t>Horodateur</t>
   </si>
@@ -1043,6 +1043,18 @@
   </si>
   <si>
     <t>Je ressens profondément le fait d'être une bulle, une bulle confortable et consensuelle, vis à vis de mon militantisme écologique. Je pense que j'ai une forme de fracture dans mon esprit que les contestations sociales représentées par le mouvement des gilets jaunes contribuent à rendre plus intelligibles, que j'arrive de mieux à mieux à appréhender et à verbaliser. Ça me donne le sentiment que je me suis trompée de combat avec le militantisme écologique et que la crise sociale est bien plus urgente pour l'humanité.</t>
+  </si>
+  <si>
+    <t>Je partage des liens sur les réseaux sociaux, Je fais profil bas. Trop en parler, c'est devenir prêcheur, et donc desservir la cause., Je donne une conférence sur les enjeux énergie-climat (hi hi hi)</t>
+  </si>
+  <si>
+    <t>Génie électrique</t>
+  </si>
+  <si>
+    <t>Je partage des liens sur les réseaux sociaux, Je partage des références directement à mon entourage (mail, vive voix etc.), Je donne une conférence sur les enjeux énergie-climat (hi hi hi), Je montre l'exemple, je suscite l'étonnement</t>
+  </si>
+  <si>
+    <t>Une religion c'est entre autre fait pour expliquer la mort, la vie après, la réincarnation etc. Avec l'écologie on parle de tout sauf d'une vie meilleure après la mort.</t>
   </si>
 </sst>
 </file>
@@ -6531,6 +6543,169 @@
         <v>59</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" s="2">
+        <v>43550.947415567134</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K67" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="L67" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="M67" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N67" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="O67" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="S67" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T67" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="U67" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V67" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="W67" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="X67" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y67" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB67" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2">
+        <v>43551.650507453705</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D68" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K68" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="L68" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="M68" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="N68" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="O68" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="R68" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="S68" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T68" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="U68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W68" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z68" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB68" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>